<commit_message>
feat: adiciona planilha com dados normalizados das musicas favoritas
</commit_message>
<xml_diff>
--- a/spotify_clone_normalizada.xlsx
+++ b/spotify_clone_normalizada.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="pessoa_usuaria" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,6 +15,7 @@
     <sheet name="musica" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="album" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="seguindo_artista" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="musica_favorita" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="87">
   <si>
     <t xml:space="preserve">pessoa_usuaria_id</t>
   </si>
@@ -297,7 +298,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -327,12 +328,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -377,7 +372,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -387,22 +382,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,14 +405,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,23 +414,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FF272727"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -470,11 +424,11 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.64"/>
@@ -492,183 +446,183 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="7" t="n">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="n">
         <v>82</v>
       </c>
-      <c r="D2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="D2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="D3" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="D4" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="3" t="n">
         <v>46</v>
       </c>
-      <c r="D5" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="D6" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="D7" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="D8" s="8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="3" t="n">
         <v>85</v>
       </c>
-      <c r="D9" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="8" t="s">
+      <c r="D9" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="n">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="3" t="n">
         <v>45</v>
       </c>
-      <c r="D10" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="n">
+      <c r="A11" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="3" t="n">
         <v>58</v>
       </c>
-      <c r="D11" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" s="8" t="s">
+      <c r="D11" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -694,7 +648,7 @@
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.61"/>
@@ -702,13 +656,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
@@ -716,7 +670,7 @@
       <c r="A2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -727,7 +681,7 @@
       <c r="A3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="0" t="n">
@@ -738,7 +692,7 @@
       <c r="A4" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C4" s="0" t="n">
@@ -749,7 +703,7 @@
       <c r="A5" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="C5" s="0" t="n">
@@ -778,17 +732,17 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.57"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
       <c r="AMH1" s="0"/>
@@ -844,34 +798,34 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="10"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8"/>
+      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -895,7 +849,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.22"/>
@@ -903,10 +857,10 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -914,178 +868,178 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="n">
+      <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="n">
+      <c r="A5" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="12" t="n">
+      <c r="A6" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="12" t="n">
+      <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="n">
+      <c r="A8" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="7" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="n">
+      <c r="A9" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="n">
+      <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="n">
+      <c r="A11" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="12" t="n">
+      <c r="A12" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="n">
+      <c r="A13" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="n">
+      <c r="A14" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="n">
+      <c r="A15" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="n">
+      <c r="A16" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="n">
+      <c r="A17" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="7" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1108,32 +1062,32 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1308,34 +1262,34 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="8"/>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="8"/>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="8"/>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="8"/>
+      <c r="B16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="8"/>
+      <c r="B17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="8"/>
+      <c r="B18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="8"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="8"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8"/>
+      <c r="B21" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1359,9 +1313,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.46"/>
@@ -1371,125 +1325,125 @@
       <c r="A1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="11" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
+      <c r="C2" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="11" t="n">
-        <v>6</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="A5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C6" s="11" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="n">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="n">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="11" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1515,17 +1469,17 @@
       <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.96"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="ALZ1" s="0"/>
@@ -1666,4 +1620,160 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="54.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.88"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>